<commit_message>
add Api, edit Vue homeView.vue
</commit_message>
<xml_diff>
--- a/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\FrontEnd\Lucas\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC13A2E8-0DE5-49B8-A186-19AAEA7FC68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B176A59C-4F81-43D0-A6B6-2D4AC73133C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Faire la partie auteur dans le home html css</t>
+  </si>
+  <si>
+    <t>explication 2 test formatifs</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -631,7 +634,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C495)</f>
-        <v>9.4444444444444442E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -757,14 +760,22 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="str">
+      <c r="A11" s="15">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45418</v>
+      </c>
+      <c r="C11" s="23">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6234,6 +6245,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6456,27 +6487,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6493,23 +6523,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Make the author fk route work
</commit_message>
<xml_diff>
--- a/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\FrontEnd\Lucas\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D787B5C-99D1-4284-A041-A2CE4A79746A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1FAF05-629E-42DD-894E-992E05F6DC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Discution avec Sofiene sur l'avancer du projet et les taches à faires</t>
+  </si>
+  <si>
+    <t>réglé les problème d'importation des données (je vérifiait que book mais pas author +JWT)</t>
+  </si>
+  <si>
+    <t>finir l'import des data sur la home page + modifier le code du header afin d'y integrer un menu déroulant</t>
+  </si>
+  <si>
+    <t>Discution de la répartition des tache ave sofienne + auto éval avec Mveng</t>
   </si>
 </sst>
 </file>
@@ -578,7 +587,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -643,7 +652,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C495)</f>
-        <v>0.18611111111111109</v>
+        <v>0.28888888888888886</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -828,36 +837,60 @@
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="str">
+      <c r="A14" s="15">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="str">
+      <c r="A15" s="15">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45425</v>
+      </c>
+      <c r="C15" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="str">
+      <c r="A16" s="15">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45426</v>
+      </c>
+      <c r="C16" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -6272,6 +6305,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -6280,15 +6322,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6515,20 +6548,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
edit Api and make the home button work
</commit_message>
<xml_diff>
--- a/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/FrontEnd/Lucas/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\FrontEnd\Lucas\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE4A17-DCF3-4BC3-80EB-8E37AF5740B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE2B494-113F-4A34-8E83-40C224F5685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Tuto suivit : https://www.youtube.com/watch?v=CgMD6VykQXQ&amp;ab_channel=CodingwithKazim                 https://www.youtube.com/watch?v=VqnJwh6E9ak&amp;t=12s&amp;ab_channel=Academind            https://www.youtube.com/watch?v=0gWd-AS4cfY&amp;ab_channel=TechnicalRajni</t>
+  </si>
+  <si>
+    <t>Introduction du cour ( discution rendu projet )</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -667,7 +670,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C495)</f>
-        <v>0.42638888888888882</v>
+        <v>0.43402777777777768</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -970,14 +973,22 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="str">
+      <c r="A20" s="15">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45440</v>
+      </c>
+      <c r="C20" s="23">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,26 +6359,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6590,10 +6581,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6610,20 +6632,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>